<commit_message>
+ NEW: cart cart in exel in TG synchronization
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Товар</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>Стоимость</t>
+  </si>
+  <si>
+    <t>ыы</t>
+  </si>
+  <si>
+    <t>2 шт</t>
   </si>
   <si>
     <t>ИТОГО:</t>
@@ -71,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -95,8 +101,22 @@
       <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
+      <c r="B2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>5</v>
+      </c>
       <c r="D2" t="n" s="0">
-        <v>0.0</v>
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>40.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>